<commit_message>
update auto scale CH2&CH3
</commit_message>
<xml_diff>
--- a/Data/SPIV_Setting _Thomas_20221213_ver0.1.0.xlsx
+++ b/Data/SPIV_Setting _Thomas_20221213_ver0.1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\OneDrive - Wistron Corporation\SIV-POWER\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A84963-F06D-449B-85FE-164532BFC05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52073AF-9769-4A29-B1BF-1D41BD05BD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3267" yWindow="1800" windowWidth="20173" windowHeight="10313" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5380" yWindow="40" windowWidth="19200" windowHeight="10073" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regulation" sheetId="5" r:id="rId1"/>
@@ -741,7 +741,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -784,42 +784,39 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="116">
@@ -1250,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.7"/>
@@ -1425,9 +1422,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="11"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1440,7 +1434,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="A4" sqref="A4:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.7"/>
@@ -1529,7 +1523,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="A6" sqref="A6:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.7"/>
@@ -1648,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="16.7"/>
@@ -1659,7 +1653,7 @@
     <col min="1" max="1" width="12.64453125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1685,7 +1679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
@@ -1696,7 +1690,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" s="9" t="s">
         <v>31</v>
       </c>
@@ -1707,7 +1701,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4" s="9" t="s">
         <v>32</v>
       </c>
@@ -1718,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8">
       <c r="A5" s="9" t="s">
         <v>33</v>
       </c>
@@ -1728,9 +1722,6 @@
       <c r="C5" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="I14" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1743,7 +1734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998D04A5-7AB6-43AC-ACC4-7E037A656E2F}">
   <dimension ref="A1:AV134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1770,56 +1761,56 @@
       <c r="B1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="S1" s="14" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="S1" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AD1" s="14" t="s">
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AD1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14"/>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AO1" s="14" t="s">
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AO1" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14"/>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
     </row>
     <row r="2" spans="1:48">
       <c r="A2" s="12" t="s">
@@ -1959,51 +1950,49 @@
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
-      <c r="AO3" s="24"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="26"/>
-      <c r="AV3" s="26"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
     </row>
     <row r="4" spans="1:48">
       <c r="A4" s="12" t="s">
@@ -2030,336 +2019,336 @@
       </c>
     </row>
     <row r="7" spans="1:48">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:48">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:48">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:48">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:48">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:48">
-      <c r="A12" s="16"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:48">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="13"/>
     </row>
     <row r="14" spans="1:48">
-      <c r="A14" s="17"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:48">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="13"/>
     </row>
     <row r="16" spans="1:48">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="13"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="13"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="13"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="13"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="13"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="13"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="13"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="14"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="14"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="14"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="19"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="13"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="19"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="13"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="19"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="13"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="19"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="13"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="19"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="13"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="19"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="13"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="19"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="13"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="19"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="13"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="19"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="13"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="19"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="13"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="20"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="13"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="20"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="13"/>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="20"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="13"/>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="20"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="13"/>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="13"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="20"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="13"/>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="20"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="13"/>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="13"/>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="20"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="13"/>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="20"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="13"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="21"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="13"/>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="21"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="14"/>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="21"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="14"/>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="21"/>
-      <c r="B49" s="15"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="14"/>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="21"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="14"/>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="21"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="14"/>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="15"/>
+      <c r="A52" s="20"/>
+      <c r="B52" s="14"/>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="15"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="14"/>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="21"/>
-      <c r="B54" s="15"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="14"/>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="21"/>
-      <c r="B55" s="15"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="14"/>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="21"/>
-      <c r="B56" s="15"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="14"/>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="21"/>
-      <c r="B57" s="15"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="14"/>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="21"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="14"/>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="21"/>
-      <c r="B59" s="15"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="14"/>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="21"/>
-      <c r="B60" s="15"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="14"/>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="21"/>
-      <c r="B61" s="15"/>
+      <c r="A61" s="20"/>
+      <c r="B61" s="14"/>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="21"/>
-      <c r="B62" s="15"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="14"/>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="21"/>
-      <c r="B63" s="15"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="14"/>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="21"/>
-      <c r="B64" s="15"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="14"/>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="21"/>
-      <c r="B65" s="15"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="14"/>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="21"/>
-      <c r="B66" s="15"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="14"/>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="21"/>
-      <c r="B67" s="15"/>
+      <c r="A67" s="20"/>
+      <c r="B67" s="14"/>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="21"/>
-      <c r="B68" s="15"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="14"/>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="21"/>
-      <c r="B69" s="15"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="14"/>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="21"/>
-      <c r="B70" s="15"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="14"/>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="21"/>
-      <c r="B71" s="15"/>
+      <c r="A71" s="20"/>
+      <c r="B71" s="14"/>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="21"/>
-      <c r="B72" s="15"/>
+      <c r="A72" s="20"/>
+      <c r="B72" s="14"/>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="21"/>
-      <c r="B73" s="15"/>
+      <c r="A73" s="20"/>
+      <c r="B73" s="14"/>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="21"/>
-      <c r="B74" s="15"/>
+      <c r="A74" s="20"/>
+      <c r="B74" s="14"/>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="21"/>
-      <c r="B75" s="15"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="14"/>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="21"/>
-      <c r="B76" s="15"/>
+      <c r="A76" s="20"/>
+      <c r="B76" s="14"/>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="21"/>
-      <c r="B77" s="15"/>
+      <c r="A77" s="20"/>
+      <c r="B77" s="14"/>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="21"/>
-      <c r="B78" s="15"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="14"/>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="21"/>
-      <c r="B79" s="15"/>
+      <c r="A79" s="20"/>
+      <c r="B79" s="14"/>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="21"/>
-      <c r="B80" s="15"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="14"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="21"/>
-      <c r="B81" s="15"/>
+      <c r="A81" s="20"/>
+      <c r="B81" s="14"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="21"/>
-      <c r="B82" s="15"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="14"/>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="21"/>
-      <c r="B83" s="15"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="14"/>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="21"/>
-      <c r="B84" s="15"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="14"/>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="21"/>
-      <c r="B85" s="15"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="14"/>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="12"/>
@@ -2482,74 +2471,74 @@
       <c r="B115" s="13"/>
     </row>
     <row r="116" spans="1:2">
-      <c r="A116" s="22"/>
-      <c r="B116" s="23"/>
+      <c r="A116" s="21"/>
+      <c r="B116" s="22"/>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="22"/>
-      <c r="B117" s="23"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="22"/>
     </row>
     <row r="118" spans="1:2">
-      <c r="A118" s="22"/>
-      <c r="B118" s="23"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="22"/>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="22"/>
-      <c r="B119" s="23"/>
+      <c r="A119" s="21"/>
+      <c r="B119" s="22"/>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="22"/>
-      <c r="B120" s="23"/>
+      <c r="A120" s="21"/>
+      <c r="B120" s="22"/>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="22"/>
-      <c r="B121" s="23"/>
+      <c r="A121" s="21"/>
+      <c r="B121" s="22"/>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="22"/>
-      <c r="B122" s="23"/>
+      <c r="A122" s="21"/>
+      <c r="B122" s="22"/>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="22"/>
-      <c r="B123" s="23"/>
+      <c r="A123" s="21"/>
+      <c r="B123" s="22"/>
     </row>
     <row r="124" spans="1:2">
-      <c r="A124" s="22"/>
-      <c r="B124" s="23"/>
+      <c r="A124" s="21"/>
+      <c r="B124" s="22"/>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="22"/>
-      <c r="B125" s="23"/>
+      <c r="A125" s="21"/>
+      <c r="B125" s="22"/>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="22"/>
-      <c r="B126" s="23"/>
+      <c r="A126" s="21"/>
+      <c r="B126" s="22"/>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="22"/>
-      <c r="B127" s="23"/>
+      <c r="A127" s="21"/>
+      <c r="B127" s="22"/>
     </row>
     <row r="128" spans="1:2">
-      <c r="A128" s="22"/>
-      <c r="B128" s="23"/>
+      <c r="A128" s="21"/>
+      <c r="B128" s="22"/>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="22"/>
+      <c r="A129" s="21"/>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="22"/>
+      <c r="A130" s="21"/>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="22"/>
+      <c r="A131" s="21"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="22"/>
+      <c r="A132" s="21"/>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="22"/>
+      <c r="A133" s="21"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="22"/>
+      <c r="A134" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>